<commit_message>
added new feature of applying filter on result
</commit_message>
<xml_diff>
--- a/src/test/resources/input/product.xlsx
+++ b/src/test/resources/input/product.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="50">
   <si>
     <t>Product</t>
   </si>
@@ -149,6 +149,27 @@
   </si>
   <si>
     <t>Lenovo Ideapad S145 Intel Core I3 8th Gen 15.6-inch Thin and Light FHD Laptop ( 4GB RAM / 1TB HDD / Windows 10 Home / Grey / 1.85Kg ), 81MV0091IN</t>
+  </si>
+  <si>
+    <t>Lenovo IdeaPad S340 81VW00CVIN 15.6-inch FHD IPS Thin and Light Laptop (10th Gen CORE I5-1035G4/8GB/512GB SSD/Windows 10/Microsoft Office/Integrated Graphics), Platinum Grey</t>
+  </si>
+  <si>
+    <t>Lenovo Ideapad S145 Intel Core I3 8th Gen 15.6-inch FHD Thin and Light Laptop ( 4GB RAM / 1TB HDD / Windows 10 Home / Office Home and Student 2019 / Grey / 1.85kg ), 81MV009JIN</t>
+  </si>
+  <si>
+    <t>Lenovo Ideapad 330 AMD A6-9225 Processor 15.6-inch HD Laptop (4GB/1TB HDD/DOS/Onyx Black/2.2Kg), 81D60079IN</t>
+  </si>
+  <si>
+    <t>Lenovo Ideapad S145 81N300F2IN 15.6-inch HD Thin and Light Laptop (7th Gen A6-9225/4GB/1TB HDD/DOS/Integrated Graphics), Grey</t>
+  </si>
+  <si>
+    <t>Lenovo IdeaPad S145 AMD A6 -9225 15.6-inch HD Thin and Light Laptop (4GB/1TB/Windows 10/MS Office 2019/Textured Black/1.85Kg), 81N300B7IN</t>
+  </si>
+  <si>
+    <t>Lenovo Ideapad S145 AMD A6-9225 15.6-inch HD Thin and Light Laptop ( 4GB RAM / 1TB HDD / Windows 10 Home / Office Home and Student 2019 / Grey / 1.85kg ), 81N3004DIN</t>
+  </si>
+  <si>
+    <t>Lenovo Legion Y540 9th Gen Intel Core i5 15.6 inch FHD Gaming Laptop -Lenovo 2TB External Hard Drive</t>
   </si>
 </sst>
 </file>
@@ -512,82 +533,82 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>